<commit_message>
Update Eve's xT weights
</commit_message>
<xml_diff>
--- a/assets/xt_weights/ma2024.xlsx
+++ b/assets/xt_weights/ma2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.bischofberger\OneDrive - VfB Stuttgart 1893 AG\Desktop\code\vfb-ma-jb\assets\xt_weights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332A8070-EE04-4E6A-85E2-B77538751A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84124C-FF3B-40C6-A428-1F8B299B6996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="10074" xr2:uid="{5F72FA24-4A65-4A30-A9DF-1C78D3874B59}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="20625" xr2:uid="{5F72FA24-4A65-4A30-A9DF-1C78D3874B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -392,609 +392,609 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="P12" sqref="A1:P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2.0999999999999999E-3</v>
+        <v>2.0752100000000001E-3</v>
       </c>
       <c r="B1">
-        <v>3.5000000000000001E-3</v>
+        <v>3.4597299999999998E-3</v>
       </c>
       <c r="C1">
-        <v>3.0999999999999999E-3</v>
+        <v>3.1180299999999999E-3</v>
       </c>
       <c r="D1">
-        <v>3.8E-3</v>
+        <v>3.7811300000000002E-3</v>
       </c>
       <c r="E1">
-        <v>4.1999999999999997E-3</v>
+        <v>4.1941399999999998E-3</v>
       </c>
       <c r="F1">
-        <v>5.8999999999999999E-3</v>
+        <v>5.9175399999999998E-3</v>
       </c>
       <c r="G1">
-        <v>7.6E-3</v>
+        <v>7.6085600000000003E-3</v>
       </c>
       <c r="H1">
-        <v>8.9999999999999993E-3</v>
+        <v>8.9948500000000004E-3</v>
       </c>
       <c r="I1">
-        <v>1.2500000000000001E-2</v>
+        <v>1.24803E-2</v>
       </c>
       <c r="J1">
-        <v>1.7100000000000001E-2</v>
+        <v>1.7114130000000002E-2</v>
       </c>
       <c r="K1">
-        <v>2.4299999999999999E-2</v>
+        <v>2.4268979999999999E-2</v>
       </c>
       <c r="L1">
-        <v>3.2500000000000001E-2</v>
+        <v>3.2517360000000002E-2</v>
       </c>
       <c r="M1">
-        <v>4.3099999999999999E-2</v>
+        <v>4.3053300000000003E-2</v>
       </c>
       <c r="N1">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2015939999999997E-2</v>
       </c>
       <c r="O1">
-        <v>5.96E-2</v>
+        <v>5.9550440000000003E-2</v>
       </c>
       <c r="P1">
-        <v>9.64E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>9.6368529999999994E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2.2000000000000001E-3</v>
+        <v>2.1810200000000001E-3</v>
       </c>
       <c r="B2">
-        <v>2.5000000000000001E-3</v>
+        <v>2.5269300000000001E-3</v>
       </c>
       <c r="C2">
-        <v>3.2000000000000002E-3</v>
+        <v>3.1884299999999999E-3</v>
       </c>
       <c r="D2">
-        <v>3.2000000000000002E-3</v>
+        <v>3.7617800000000002E-3</v>
       </c>
       <c r="E2">
-        <v>4.5999999999999999E-3</v>
+        <v>4.6471500000000001E-3</v>
       </c>
       <c r="F2">
-        <v>6.0000000000000001E-3</v>
+        <v>6.0253199999999998E-3</v>
       </c>
       <c r="G2">
-        <v>8.8000000000000005E-3</v>
+        <v>8.8139900000000007E-3</v>
       </c>
       <c r="H2">
-        <v>1.0699999999999999E-2</v>
+        <v>1.069781E-2</v>
       </c>
       <c r="I2">
-        <v>1.49E-2</v>
+        <v>1.4852539999999999E-2</v>
       </c>
       <c r="J2">
-        <v>1.49E-2</v>
+        <v>1.8775099999999999E-2</v>
       </c>
       <c r="K2">
-        <v>2.5899999999999999E-2</v>
+        <v>2.5881609999999999E-2</v>
       </c>
       <c r="L2">
-        <v>3.49E-2</v>
+        <v>3.4921569999999999E-2</v>
       </c>
       <c r="M2">
-        <v>4.6899999999999997E-2</v>
+        <v>4.6905269999999999E-2</v>
       </c>
       <c r="N2">
-        <v>5.8299999999999998E-2</v>
+        <v>5.8328150000000002E-2</v>
       </c>
       <c r="O2">
-        <v>7.3800000000000004E-2</v>
+        <v>7.3821750000000005E-2</v>
       </c>
       <c r="P2">
-        <v>7.8700000000000006E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>7.87471E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2.3999999999999998E-3</v>
+        <v>2.4161E-3</v>
       </c>
       <c r="B3">
-        <v>2.8999999999999998E-3</v>
+        <v>2.9176100000000002E-3</v>
       </c>
       <c r="C3">
-        <v>3.3E-3</v>
+        <v>3.2614599999999999E-3</v>
       </c>
       <c r="D3">
-        <v>3.3E-3</v>
+        <v>3.9478300000000003E-3</v>
       </c>
       <c r="E3">
-        <v>5.3E-3</v>
+        <v>5.3288199999999997E-3</v>
       </c>
       <c r="F3">
-        <v>6.6E-3</v>
+        <v>6.5605200000000002E-3</v>
       </c>
       <c r="G3">
-        <v>8.8000000000000005E-3</v>
+        <v>8.79454E-3</v>
       </c>
       <c r="H3">
-        <v>1.1599999999999999E-2</v>
+        <v>1.1604919999999999E-2</v>
       </c>
       <c r="I3">
-        <v>1.54E-2</v>
+        <v>1.541873E-2</v>
       </c>
       <c r="J3">
-        <v>1.54E-2</v>
+        <v>1.99995E-2</v>
       </c>
       <c r="K3">
-        <v>2.7300000000000001E-2</v>
+        <v>2.7287949999999998E-2</v>
       </c>
       <c r="L3">
-        <v>3.7900000000000003E-2</v>
+        <v>3.7895270000000002E-2</v>
       </c>
       <c r="M3">
-        <v>5.1999999999999998E-2</v>
+        <v>5.1958310000000001E-2</v>
       </c>
       <c r="N3">
-        <v>6.1199999999999997E-2</v>
+        <v>6.1233089999999997E-2</v>
       </c>
       <c r="O3">
-        <v>7.3400000000000007E-2</v>
+        <v>7.3374110000000006E-2</v>
       </c>
       <c r="P3">
-        <v>0.1051</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>0.10512987999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.5000000000000001E-3</v>
+        <v>2.5145599999999999E-3</v>
       </c>
       <c r="B4">
-        <v>3.0000000000000001E-3</v>
+        <v>3.0387600000000002E-3</v>
       </c>
       <c r="C4">
-        <v>3.5000000000000001E-3</v>
+        <v>3.4647499999999999E-3</v>
       </c>
       <c r="D4">
-        <v>3.5000000000000001E-3</v>
+        <v>3.9421899999999999E-3</v>
       </c>
       <c r="E4">
-        <v>5.1999999999999998E-3</v>
+        <v>5.1849399999999999E-3</v>
       </c>
       <c r="F4">
-        <v>6.7999999999999996E-3</v>
+        <v>6.7616100000000004E-3</v>
       </c>
       <c r="G4">
-        <v>9.4999999999999998E-3</v>
+        <v>9.47747E-3</v>
       </c>
       <c r="H4">
-        <v>1.24E-2</v>
+        <v>1.237365E-2</v>
       </c>
       <c r="I4">
-        <v>1.66E-2</v>
+        <v>1.6581700000000001E-2</v>
       </c>
       <c r="J4">
-        <v>1.66E-2</v>
+        <v>2.1697250000000001E-2</v>
       </c>
       <c r="K4">
-        <v>3.0200000000000001E-2</v>
+        <v>3.0165549999999999E-2</v>
       </c>
       <c r="L4">
-        <v>3.9899999999999998E-2</v>
+        <v>3.9909449999999999E-2</v>
       </c>
       <c r="M4">
-        <v>5.16E-2</v>
+        <v>5.1645360000000001E-2</v>
       </c>
       <c r="N4">
-        <v>6.2199999999999998E-2</v>
+        <v>6.222155E-2</v>
       </c>
       <c r="O4">
-        <v>7.5899999999999995E-2</v>
+        <v>7.5899900000000006E-2</v>
       </c>
       <c r="P4">
-        <v>9.7699999999999995E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>9.7732079999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.8999999999999998E-3</v>
+        <v>2.9393900000000001E-3</v>
       </c>
       <c r="B5">
-        <v>3.2000000000000002E-3</v>
+        <v>3.1586499999999998E-3</v>
       </c>
       <c r="C5">
-        <v>3.7000000000000002E-3</v>
+        <v>3.74947E-3</v>
       </c>
       <c r="D5">
-        <v>3.7000000000000002E-3</v>
+        <v>4.4350600000000002E-3</v>
       </c>
       <c r="E5">
-        <v>5.4999999999999997E-3</v>
+        <v>5.5188099999999999E-3</v>
       </c>
       <c r="F5">
-        <v>6.8999999999999999E-3</v>
+        <v>6.9255000000000002E-3</v>
       </c>
       <c r="G5">
-        <v>9.4999999999999998E-3</v>
+        <v>9.5269299999999994E-3</v>
       </c>
       <c r="H5">
-        <v>1.2500000000000001E-2</v>
+        <v>1.24624E-2</v>
       </c>
       <c r="I5">
-        <v>1.6500000000000001E-2</v>
+        <v>1.6496830000000001E-2</v>
       </c>
       <c r="J5">
-        <v>1.6500000000000001E-2</v>
+        <v>2.2555599999999999E-2</v>
       </c>
       <c r="K5">
-        <v>3.04E-2</v>
+        <v>3.0357249999999999E-2</v>
       </c>
       <c r="L5">
-        <v>3.9699999999999999E-2</v>
+        <v>3.972009E-2</v>
       </c>
       <c r="M5">
-        <v>5.1999999999999998E-2</v>
+        <v>5.195553E-2</v>
       </c>
       <c r="N5">
-        <v>7.3800000000000004E-2</v>
+        <v>7.3791209999999996E-2</v>
       </c>
       <c r="O5">
-        <v>0.1077</v>
+        <v>0.1077317</v>
       </c>
       <c r="P5">
-        <v>0.1119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1119124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4.8999999999999998E-3</v>
+        <v>4.8831100000000004E-3</v>
       </c>
       <c r="B6">
-        <v>3.5000000000000001E-3</v>
+        <v>3.52294E-3</v>
       </c>
       <c r="C6">
-        <v>4.1999999999999997E-3</v>
+        <v>4.2066500000000001E-3</v>
       </c>
       <c r="D6">
-        <v>4.1999999999999997E-3</v>
+        <v>4.4654100000000004E-3</v>
       </c>
       <c r="E6">
-        <v>5.3E-3</v>
+        <v>5.2741300000000001E-3</v>
       </c>
       <c r="F6">
-        <v>7.1999999999999998E-3</v>
+        <v>7.1613400000000004E-3</v>
       </c>
       <c r="G6">
-        <v>9.2999999999999992E-3</v>
+        <v>9.2518400000000008E-3</v>
       </c>
       <c r="H6">
-        <v>1.21E-2</v>
+        <v>1.2123480000000001E-2</v>
       </c>
       <c r="I6">
-        <v>1.5599999999999999E-2</v>
+        <v>1.561274E-2</v>
       </c>
       <c r="J6">
-        <v>1.5599999999999999E-2</v>
+        <v>2.2309530000000001E-2</v>
       </c>
       <c r="K6">
-        <v>0.03</v>
+        <v>3.0049960000000001E-2</v>
       </c>
       <c r="L6">
-        <v>3.9300000000000002E-2</v>
+        <v>3.9341309999999997E-2</v>
       </c>
       <c r="M6">
-        <v>5.1700000000000003E-2</v>
+        <v>5.1656229999999997E-2</v>
       </c>
       <c r="N6">
-        <v>8.0299999999999996E-2</v>
+        <v>8.0267809999999995E-2</v>
       </c>
       <c r="O6">
-        <v>0.13769999999999999</v>
+        <v>0.13767861000000001</v>
       </c>
       <c r="P6">
-        <v>0.27789999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>0.27787431000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5.0000000000000001E-3</v>
+        <v>5.01243E-3</v>
       </c>
       <c r="B7">
-        <v>3.5000000000000001E-3</v>
+        <v>3.5446800000000001E-3</v>
       </c>
       <c r="C7">
-        <v>4.0000000000000001E-3</v>
+        <v>3.9897099999999996E-3</v>
       </c>
       <c r="D7">
-        <v>4.0000000000000001E-3</v>
+        <v>4.5773599999999999E-3</v>
       </c>
       <c r="E7">
-        <v>5.5999999999999999E-3</v>
+        <v>5.5795100000000002E-3</v>
       </c>
       <c r="F7">
-        <v>6.8999999999999999E-3</v>
+        <v>6.8592799999999997E-3</v>
       </c>
       <c r="G7">
-        <v>9.4000000000000004E-3</v>
+        <v>9.4482400000000001E-3</v>
       </c>
       <c r="H7">
-        <v>1.23E-2</v>
+        <v>1.234231E-2</v>
       </c>
       <c r="I7">
-        <v>1.5599999999999999E-2</v>
+        <v>1.559347E-2</v>
       </c>
       <c r="J7">
-        <v>1.5599999999999999E-2</v>
+        <v>2.2097149999999999E-2</v>
       </c>
       <c r="K7">
-        <v>3.1800000000000002E-2</v>
+        <v>3.1751910000000001E-2</v>
       </c>
       <c r="L7">
-        <v>3.78E-2</v>
+        <v>3.7778119999999998E-2</v>
       </c>
       <c r="M7">
-        <v>5.0299999999999997E-2</v>
+        <v>5.0324149999999998E-2</v>
       </c>
       <c r="N7">
-        <v>8.0799999999999997E-2</v>
+        <v>8.0801120000000004E-2</v>
       </c>
       <c r="O7">
-        <v>0.1396</v>
+        <v>0.13963702</v>
       </c>
       <c r="P7">
-        <v>0.32679999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>0.32677356000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2.7000000000000001E-3</v>
+        <v>2.7136500000000002E-3</v>
       </c>
       <c r="B8">
-        <v>3.5000000000000001E-3</v>
+        <v>3.51323E-3</v>
       </c>
       <c r="C8">
-        <v>3.5999999999999999E-3</v>
+        <v>3.5880199999999999E-3</v>
       </c>
       <c r="D8">
-        <v>3.5999999999999999E-3</v>
+        <v>4.6043799999999999E-3</v>
       </c>
       <c r="E8">
-        <v>5.5999999999999999E-3</v>
+        <v>5.5725000000000002E-3</v>
       </c>
       <c r="F8">
-        <v>7.0000000000000001E-3</v>
+        <v>7.0460100000000001E-3</v>
       </c>
       <c r="G8">
-        <v>9.4999999999999998E-3</v>
+        <v>9.4685199999999994E-3</v>
       </c>
       <c r="H8">
-        <v>1.2800000000000001E-2</v>
+        <v>1.2811940000000001E-2</v>
       </c>
       <c r="I8">
-        <v>1.6299999999999999E-2</v>
+        <v>1.6255889999999999E-2</v>
       </c>
       <c r="J8">
-        <v>1.6299999999999999E-2</v>
+        <v>2.1804589999999999E-2</v>
       </c>
       <c r="K8">
-        <v>3.04E-2</v>
+        <v>3.03643E-2</v>
       </c>
       <c r="L8">
-        <v>4.0099999999999997E-2</v>
+        <v>4.0082710000000001E-2</v>
       </c>
       <c r="M8">
-        <v>5.0700000000000002E-2</v>
+        <v>5.0715509999999998E-2</v>
       </c>
       <c r="N8">
-        <v>7.1300000000000002E-2</v>
+        <v>7.1279480000000006E-2</v>
       </c>
       <c r="O8">
-        <v>0.1089</v>
+        <v>0.10886009000000001</v>
       </c>
       <c r="P8">
-        <v>9.9099999999999994E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>9.9103060000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2.7000000000000001E-3</v>
+        <v>2.7469999999999999E-3</v>
       </c>
       <c r="B9">
-        <v>3.3E-3</v>
+        <v>3.2672299999999999E-3</v>
       </c>
       <c r="C9">
-        <v>3.2000000000000002E-3</v>
+        <v>3.2147199999999999E-3</v>
       </c>
       <c r="D9">
-        <v>3.2000000000000002E-3</v>
+        <v>3.9407799999999996E-3</v>
       </c>
       <c r="E9">
-        <v>5.1999999999999998E-3</v>
+        <v>5.1883700000000003E-3</v>
       </c>
       <c r="F9">
-        <v>6.7999999999999996E-3</v>
+        <v>6.7784500000000001E-3</v>
       </c>
       <c r="G9">
-        <v>9.2999999999999992E-3</v>
+        <v>9.3439700000000001E-3</v>
       </c>
       <c r="H9">
-        <v>1.2500000000000001E-2</v>
+        <v>1.254736E-2</v>
       </c>
       <c r="I9">
-        <v>1.61E-2</v>
+        <v>1.6093489999999998E-2</v>
       </c>
       <c r="J9">
-        <v>1.61E-2</v>
+        <v>2.1886599999999999E-2</v>
       </c>
       <c r="K9">
-        <v>2.9399999999999999E-2</v>
+        <v>2.939742E-2</v>
       </c>
       <c r="L9">
-        <v>3.8899999999999997E-2</v>
+        <v>3.8915270000000002E-2</v>
       </c>
       <c r="M9">
-        <v>5.0999999999999997E-2</v>
+        <v>5.101257E-2</v>
       </c>
       <c r="N9">
-        <v>6.1400000000000003E-2</v>
+        <v>6.1392229999999999E-2</v>
       </c>
       <c r="O9">
-        <v>8.4599999999999995E-2</v>
+        <v>8.461349E-2</v>
       </c>
       <c r="P9">
-        <v>9.6000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>9.604886E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2.3E-3</v>
+        <v>2.2759799999999999E-3</v>
       </c>
       <c r="B10">
-        <v>2.8E-3</v>
+        <v>2.8146E-3</v>
       </c>
       <c r="C10">
-        <v>3.0999999999999999E-3</v>
+        <v>3.1499499999999999E-3</v>
       </c>
       <c r="D10">
-        <v>3.0999999999999999E-3</v>
+        <v>4.0112500000000001E-3</v>
       </c>
       <c r="E10">
-        <v>4.8999999999999998E-3</v>
+        <v>4.8996899999999999E-3</v>
       </c>
       <c r="F10">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3712899999999999E-3</v>
       </c>
       <c r="G10">
-        <v>8.5000000000000006E-3</v>
+        <v>8.4970400000000008E-3</v>
       </c>
       <c r="H10">
-        <v>1.1299999999999999E-2</v>
+        <v>1.132233E-2</v>
       </c>
       <c r="I10">
-        <v>1.54E-2</v>
+        <v>1.5384109999999999E-2</v>
       </c>
       <c r="J10">
-        <v>1.54E-2</v>
+        <v>2.0852099999999998E-2</v>
       </c>
       <c r="K10">
-        <v>2.8500000000000001E-2</v>
+        <v>2.8474200000000002E-2</v>
       </c>
       <c r="L10">
-        <v>3.8399999999999997E-2</v>
+        <v>3.8444470000000001E-2</v>
       </c>
       <c r="M10">
-        <v>5.0200000000000002E-2</v>
+        <v>5.0209509999999999E-2</v>
       </c>
       <c r="N10">
-        <v>6.2899999999999998E-2</v>
+        <v>6.2861299999999995E-2</v>
       </c>
       <c r="O10">
-        <v>7.9100000000000004E-2</v>
+        <v>7.906929E-2</v>
       </c>
       <c r="P10">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>9.4031939999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2.0999999999999999E-3</v>
+        <v>2.1414699999999999E-3</v>
       </c>
       <c r="B11">
-        <v>2.5000000000000001E-3</v>
+        <v>2.46831E-3</v>
       </c>
       <c r="C11">
-        <v>3.0000000000000001E-3</v>
+        <v>3.0158899999999998E-3</v>
       </c>
       <c r="D11">
-        <v>3.0000000000000001E-3</v>
+        <v>3.5001099999999999E-3</v>
       </c>
       <c r="E11">
-        <v>4.8999999999999998E-3</v>
+        <v>4.9330700000000003E-3</v>
       </c>
       <c r="F11">
-        <v>5.7999999999999996E-3</v>
+        <v>5.8068E-3</v>
       </c>
       <c r="G11">
-        <v>8.3999999999999995E-3</v>
+        <v>8.3581999999999997E-3</v>
       </c>
       <c r="H11">
-        <v>1.03E-2</v>
+        <v>1.027309E-2</v>
       </c>
       <c r="I11">
-        <v>1.43E-2</v>
+        <v>1.4333159999999999E-2</v>
       </c>
       <c r="J11">
-        <v>1.43E-2</v>
+        <v>1.8011280000000001E-2</v>
       </c>
       <c r="K11">
-        <v>2.5399999999999999E-2</v>
+        <v>2.5439949999999999E-2</v>
       </c>
       <c r="L11">
-        <v>3.3000000000000002E-2</v>
+        <v>3.3047060000000003E-2</v>
       </c>
       <c r="M11">
-        <v>4.4600000000000001E-2</v>
+        <v>4.4588700000000002E-2</v>
       </c>
       <c r="N11">
-        <v>5.6399999999999999E-2</v>
+        <v>5.638315E-2</v>
       </c>
       <c r="O11">
-        <v>6.7100000000000007E-2</v>
+        <v>6.7055030000000002E-2</v>
       </c>
       <c r="P11">
-        <v>7.5899999999999995E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+        <v>7.5883889999999996E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2.5000000000000001E-3</v>
+        <v>2.52185E-3</v>
       </c>
       <c r="B12">
-        <v>2.8E-3</v>
+        <v>2.8233199999999998E-3</v>
       </c>
       <c r="C12">
-        <v>3.5000000000000001E-3</v>
+        <v>3.5152899999999999E-3</v>
       </c>
       <c r="D12">
-        <v>3.5000000000000001E-3</v>
+        <v>3.5638000000000002E-3</v>
       </c>
       <c r="E12">
-        <v>4.3E-3</v>
+        <v>4.3325500000000001E-3</v>
       </c>
       <c r="F12">
-        <v>6.0000000000000001E-3</v>
+        <v>5.9919700000000001E-3</v>
       </c>
       <c r="G12">
-        <v>7.3000000000000001E-3</v>
+        <v>7.2857E-3</v>
       </c>
       <c r="H12">
-        <v>0.01</v>
+        <v>1.002957E-2</v>
       </c>
       <c r="I12">
-        <v>1.32E-2</v>
+        <v>1.323617E-2</v>
       </c>
       <c r="J12">
-        <v>1.32E-2</v>
+        <v>1.7077330000000002E-2</v>
       </c>
       <c r="K12">
-        <v>2.4E-2</v>
+        <v>2.395721E-2</v>
       </c>
       <c r="L12">
-        <v>3.2199999999999999E-2</v>
+        <v>3.2228689999999997E-2</v>
       </c>
       <c r="M12">
-        <v>4.0599999999999997E-2</v>
+        <v>4.0616489999999998E-2</v>
       </c>
       <c r="N12">
-        <v>4.9000000000000002E-2</v>
+        <v>4.9033800000000002E-2</v>
       </c>
       <c r="O12">
-        <v>5.9900000000000002E-2</v>
+        <v>5.9930619999999997E-2</v>
       </c>
       <c r="P12">
-        <v>0.1016</v>
+        <v>0.10157423</v>
       </c>
     </row>
   </sheetData>
@@ -1010,9 +1010,9 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>21</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>22</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>24</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>25</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>29</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>49</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>2779</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>50</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>3268</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>27</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>27</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>23</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>21</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>25</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>B2/10000</f>
         <v>2.0999999999999999E-3</v>
@@ -1678,7 +1678,7 @@
         <v>9.64E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" ref="B17:Q17" si="1">B3/10000</f>
         <v>2.2000000000000001E-3</v>
@@ -1744,7 +1744,7 @@
         <v>7.8700000000000006E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" ref="B18:Q18" si="2">B4/10000</f>
         <v>2.3999999999999998E-3</v>
@@ -1810,7 +1810,7 @@
         <v>0.1051</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" ref="B19:Q19" si="3">B5/10000</f>
         <v>2.5000000000000001E-3</v>
@@ -1876,7 +1876,7 @@
         <v>9.7699999999999995E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" ref="B20:Q20" si="4">B6/10000</f>
         <v>2.8999999999999998E-3</v>
@@ -1942,7 +1942,7 @@
         <v>0.1119</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" ref="B21:Q21" si="5">B7/10000</f>
         <v>4.8999999999999998E-3</v>
@@ -2008,7 +2008,7 @@
         <v>0.27789999999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" ref="B22:Q22" si="6">B8/10000</f>
         <v>5.0000000000000001E-3</v>
@@ -2074,7 +2074,7 @@
         <v>0.32679999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" ref="B23:Q23" si="7">B9/10000</f>
         <v>2.7000000000000001E-3</v>
@@ -2140,7 +2140,7 @@
         <v>9.9099999999999994E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" ref="B24:Q24" si="8">B10/10000</f>
         <v>2.7000000000000001E-3</v>
@@ -2206,7 +2206,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" ref="B25:Q25" si="9">B11/10000</f>
         <v>2.3E-3</v>
@@ -2272,7 +2272,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" ref="B26:Q26" si="10">B12/10000</f>
         <v>2.0999999999999999E-3</v>
@@ -2338,7 +2338,7 @@
         <v>7.5899999999999995E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" ref="B27:Q27" si="11">B13/10000</f>
         <v>2.5000000000000001E-3</v>

</xml_diff>